<commit_message>
added headers to metadata
</commit_message>
<xml_diff>
--- a/data/core_publications.xlsx
+++ b/data/core_publications.xlsx
@@ -8916,12 +8916,12 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>pub.1032125823</t>
+          <t>pub.1009389919</t>
         </is>
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>05/02866 Energy consumption and GDP in developing countries: a cointegrated panel analysis</t>
+          <t>The relationship between energy consumption, energy prices and economic growth: time series evidence from Asian developing countries</t>
         </is>
       </c>
     </row>
@@ -8938,12 +8938,12 @@
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>pub.1009389919</t>
+          <t>pub.1009749897</t>
         </is>
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>The relationship between energy consumption, energy prices and economic growth: time series evidence from Asian developing countries</t>
+          <t>Energy consumption, economic growth, and carbon emissions: Challenges faced by an EU candidate member</t>
         </is>
       </c>
     </row>
@@ -8960,12 +8960,12 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>pub.1009749897</t>
+          <t>pub.1053441851</t>
         </is>
       </c>
       <c r="D388" t="inlineStr">
         <is>
-          <t>Energy consumption, economic growth, and carbon emissions: Challenges faced by an EU candidate member</t>
+          <t>Energy consumption and GDP: causality relationship in G-7 countries and emerging markets</t>
         </is>
       </c>
     </row>
@@ -8982,12 +8982,12 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>pub.1053441851</t>
+          <t>pub.1006882307</t>
         </is>
       </c>
       <c r="D389" t="inlineStr">
         <is>
-          <t>Energy consumption and GDP: causality relationship in G-7 countries and emerging markets</t>
+          <t>Energy consumption, income, and carbon emissions in the United States</t>
         </is>
       </c>
     </row>
@@ -9004,12 +9004,12 @@
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>pub.1006882307</t>
+          <t>pub.1032217726</t>
         </is>
       </c>
       <c r="D390" t="inlineStr">
         <is>
-          <t>Energy consumption, income, and carbon emissions in the United States</t>
+          <t>Energy consumption, carbon emissions, and economic growth in China</t>
         </is>
       </c>
     </row>
@@ -9026,12 +9026,12 @@
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>pub.1032217726</t>
+          <t>pub.1042544661</t>
         </is>
       </c>
       <c r="D391" t="inlineStr">
         <is>
-          <t>Energy consumption, carbon emissions, and economic growth in China</t>
+          <t>An econometric study of CO2 emissions, energy consumption, income and foreign trade in Turkey</t>
         </is>
       </c>
     </row>
@@ -9048,12 +9048,12 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>pub.1042544661</t>
+          <t>pub.1123961798</t>
         </is>
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>An econometric study of CO2 emissions, energy consumption, income and foreign trade in Turkey</t>
+          <t>Citation-based systematic literature review of energy-growth nexus: An overview of the field and content analysis of the top 50 influential papers</t>
         </is>
       </c>
     </row>
@@ -9070,12 +9070,12 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>pub.1123961798</t>
+          <t>pub.1048730269</t>
         </is>
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>Citation-based systematic literature review of energy-growth nexus: An overview of the field and content analysis of the top 50 influential papers</t>
+          <t>Energy consumption and GDP in developing countries: A cointegrated panel analysis</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed from FAISS to Chroma Added recall evaluation Added eval notebook refactored code
</commit_message>
<xml_diff>
--- a/data/core_publications.xlsx
+++ b/data/core_publications.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="1116">
   <si>
-    <t>Group</t>
+    <t>Topic</t>
   </si>
   <si>
     <t>Survey</t>
   </si>
   <si>
-    <t>Core Publications</t>
+    <t>Pub_id</t>
   </si>
   <si>
     <t>Title</t>
@@ -3379,7 +3379,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>

</xml_diff>

<commit_message>
Updated the core pubs for cloud migration
</commit_message>
<xml_diff>
--- a/data/core_publications.xlsx
+++ b/data/core_publications.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D815"/>
+  <dimension ref="A1:D809"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15538,12 +15538,12 @@
       </c>
       <c r="C687" t="inlineStr">
         <is>
-          <t>pub.1043355881</t>
+          <t>pub.1094505139</t>
         </is>
       </c>
       <c r="D687" t="inlineStr">
         <is>
-          <t>Challenges in Collaborative Modeling: A Literature Review</t>
+          <t>CDOSim: Simulating Cloud Deployment Options for Software Migration Support</t>
         </is>
       </c>
     </row>
@@ -15560,12 +15560,12 @@
       </c>
       <c r="C688" t="inlineStr">
         <is>
-          <t>pub.1036043271</t>
+          <t>pub.1094808840</t>
         </is>
       </c>
       <c r="D688" t="inlineStr">
         <is>
-          <t>An analysis of data sets used to train and validate cost prediction systems</t>
+          <t>An Extensible Architecture for Detecting Violations of a Cloud Environment&amp;#x27;s Constraints During Legacy Software System Migration</t>
         </is>
       </c>
     </row>
@@ -15582,12 +15582,12 @@
       </c>
       <c r="C689" t="inlineStr">
         <is>
-          <t>pub.1012689387</t>
+          <t>pub.1119463839</t>
         </is>
       </c>
       <c r="D689" t="inlineStr">
         <is>
-          <t>A survey and taxonomy of approaches for mining software repositories in the context of software evolution</t>
+          <t>CloudGenius: Decision Support for Web Server Cloud Migration</t>
         </is>
       </c>
     </row>
@@ -15604,12 +15604,12 @@
       </c>
       <c r="C690" t="inlineStr">
         <is>
-          <t>pub.1019803350</t>
+          <t>pub.1093694541</t>
         </is>
       </c>
       <c r="D690" t="inlineStr">
         <is>
-          <t>A Quantitative Assessment of Requirements Engineering Publications – 1963–2006</t>
+          <t>Cloudstep: A Step-by-Step Decision Process to Support Legacy Application Migration to the Cloud</t>
         </is>
       </c>
     </row>
@@ -15626,12 +15626,12 @@
       </c>
       <c r="C691" t="inlineStr">
         <is>
-          <t>pub.1095674802</t>
+          <t>pub.1094203398</t>
         </is>
       </c>
       <c r="D691" t="inlineStr">
         <is>
-          <t>A Conceptual Model of ICT-Supported Unified Process of International Outsourcing of Software Production</t>
+          <t>Software Engineering Challenges for Migration to the Service Cloud Paradigm</t>
         </is>
       </c>
     </row>
@@ -15648,12 +15648,12 @@
       </c>
       <c r="C692" t="inlineStr">
         <is>
-          <t>pub.1052578288</t>
+          <t>pub.1093422882</t>
         </is>
       </c>
       <c r="D692" t="inlineStr">
         <is>
-          <t>Quality, productivity and economic benefits of software reuse: a review of industrial studies</t>
+          <t>Cloud Migration: A Case Study of Migrating an Enterprise IT System to IaaS</t>
         </is>
       </c>
     </row>
@@ -15670,12 +15670,12 @@
       </c>
       <c r="C693" t="inlineStr">
         <is>
-          <t>pub.1031618271</t>
+          <t>pub.1026275219</t>
         </is>
       </c>
       <c r="D693" t="inlineStr">
         <is>
-          <t>Mobile Systems Development: A Literature Review</t>
+          <t>How to adapt applications for the Cloud environment</t>
         </is>
       </c>
     </row>
@@ -15692,12 +15692,12 @@
       </c>
       <c r="C694" t="inlineStr">
         <is>
-          <t>pub.1062959392</t>
+          <t>pub.1094635108</t>
         </is>
       </c>
       <c r="D694" t="inlineStr">
         <is>
-          <t>MEASUREMENT IN SOFTWARE ENGINEERING: FROM THE ROADMAP TO THE CROSSROADS</t>
+          <t>Migration of Multi-tier Applications to Infrastructure-as-a-Service Clouds: An Investigation Using Kernel-based Virtual Machines</t>
         </is>
       </c>
     </row>
@@ -15714,12 +15714,12 @@
       </c>
       <c r="C695" t="inlineStr">
         <is>
-          <t>pub.1014654869</t>
+          <t>pub.1095459235</t>
         </is>
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>In search of `architectural knowledge&amp;#x27;</t>
+          <t>Legacy Application Migration to the Cloud: Practicability and Methodology</t>
         </is>
       </c>
     </row>
@@ -15736,12 +15736,12 @@
       </c>
       <c r="C696" t="inlineStr">
         <is>
-          <t>pub.1061420973</t>
+          <t>pub.1095784692</t>
         </is>
       </c>
       <c r="D696" t="inlineStr">
         <is>
-          <t>Improving Evidence about Software Technologies: A Look at Model-Based Testing</t>
+          <t>Migration to Cloud as Real Option Investment decision under uncertainty</t>
         </is>
       </c>
     </row>
@@ -15758,12 +15758,12 @@
       </c>
       <c r="C697" t="inlineStr">
         <is>
-          <t>pub.1012774582</t>
+          <t>pub.1093590373</t>
         </is>
       </c>
       <c r="D697" t="inlineStr">
         <is>
-          <t>How Does a Measurement Programme Evolve in Software Organizations?</t>
+          <t>Migrating Service-Oriented System to Cloud Computing: An Experience Report</t>
         </is>
       </c>
     </row>
@@ -15780,12 +15780,12 @@
       </c>
       <c r="C698" t="inlineStr">
         <is>
-          <t>pub.1093218858</t>
+          <t>pub.1015329134</t>
         </is>
       </c>
       <c r="D698" t="inlineStr">
         <is>
-          <t>Experimental Context Classification: Incentives and Experience of Subjects</t>
+          <t>Cloud adoption</t>
         </is>
       </c>
     </row>
@@ -15802,12 +15802,12 @@
       </c>
       <c r="C699" t="inlineStr">
         <is>
-          <t>pub.1061788449</t>
+          <t>pub.1095092589</t>
         </is>
       </c>
       <c r="D699" t="inlineStr">
         <is>
-          <t>Evidence-based guidelines for assessment of software development cost uncertainty</t>
+          <t>Workload Migration into Clouds - Challenges, Experiences, Opportunities</t>
         </is>
       </c>
     </row>
@@ -15824,12 +15824,12 @@
       </c>
       <c r="C700" t="inlineStr">
         <is>
-          <t>pub.1095289700</t>
+          <t>pub.1031146575</t>
         </is>
       </c>
       <c r="D700" t="inlineStr">
         <is>
-          <t>Effectiveness of Requirements Elicitation Techniques: Empirical Results Derived from a Systematic Review</t>
+          <t>Application migration to cloud</t>
         </is>
       </c>
     </row>
@@ -15846,12 +15846,12 @@
       </c>
       <c r="C701" t="inlineStr">
         <is>
-          <t>pub.1033313185</t>
+          <t>pub.1029470968</t>
         </is>
       </c>
       <c r="D701" t="inlineStr">
         <is>
-          <t>Developing Open Source Software: A Community-Based Analysis of Research</t>
+          <t>A tale of migration to cloud computing for sharing experiences and observations</t>
         </is>
       </c>
     </row>
@@ -15868,12 +15868,12 @@
       </c>
       <c r="C702" t="inlineStr">
         <is>
-          <t>pub.1023990088</t>
+          <t>pub.1094056660</t>
         </is>
       </c>
       <c r="D702" t="inlineStr">
         <is>
-          <t>Data sets and data quality in software engineering</t>
+          <t>Size Estimation of Cloud Migration Projects with Cloud Migration Point (CMP)</t>
         </is>
       </c>
     </row>
@@ -15890,12 +15890,12 @@
       </c>
       <c r="C703" t="inlineStr">
         <is>
-          <t>pub.1008918541</t>
+          <t>pub.1095101569</t>
         </is>
       </c>
       <c r="D703" t="inlineStr">
         <is>
-          <t>A new research agenda for tool integration</t>
+          <t>A Practical Architecture of Cloudification of Legacy Applications</t>
         </is>
       </c>
     </row>
@@ -15912,12 +15912,12 @@
       </c>
       <c r="C704" t="inlineStr">
         <is>
-          <t>pub.1030075621</t>
+          <t>pub.1017004215</t>
         </is>
       </c>
       <c r="D704" t="inlineStr">
         <is>
-          <t>Where Is the Proof? - A Review of Experiences from Applying MDE in Industry</t>
+          <t>Automatic conformance checking for migrating software systems to cloud infrastructures and platforms</t>
         </is>
       </c>
     </row>
@@ -15934,12 +15934,12 @@
       </c>
       <c r="C705" t="inlineStr">
         <is>
-          <t>pub.1004881437</t>
+          <t>pub.1027646047</t>
         </is>
       </c>
       <c r="D705" t="inlineStr">
         <is>
-          <t>The type of evidence produced by empirical software engineers</t>
+          <t>The Cloud Adoption Toolkit: supporting cloud adoption decisions in the enterprise</t>
         </is>
       </c>
     </row>
@@ -15956,12 +15956,12 @@
       </c>
       <c r="C706" t="inlineStr">
         <is>
-          <t>pub.1061788671</t>
+          <t>pub.1063158434</t>
         </is>
       </c>
       <c r="D706" t="inlineStr">
         <is>
-          <t>The Role of Deliberate Artificial Design Elements in Software Engineering Experiments</t>
+          <t>Cloudward bound</t>
         </is>
       </c>
     </row>
@@ -15978,144 +15978,144 @@
       </c>
       <c r="C707" t="inlineStr">
         <is>
-          <t>pub.1049407720</t>
+          <t>pub.1095280257</t>
         </is>
       </c>
       <c r="D707" t="inlineStr">
         <is>
-          <t>Techniques for developing more accessible web applications</t>
+          <t>Search-Based Genetic Optimization for Deployment and Reconfiguration of Software in the Cloud</t>
         </is>
       </c>
     </row>
     <row r="708">
       <c r="A708" t="inlineStr">
         <is>
-          <t>Cloud Migration</t>
+          <t>Software Fault Prediction Metrics</t>
         </is>
       </c>
       <c r="B708" t="inlineStr">
         <is>
-          <t>pub.1061541753</t>
+          <t>pub.1038168456</t>
         </is>
       </c>
       <c r="C708" t="inlineStr">
         <is>
-          <t>pub.1011427038</t>
+          <t>pub.1095624517</t>
         </is>
       </c>
       <c r="D708" t="inlineStr">
         <is>
-          <t>Tailoring and Introduction of the Rational Unified Process</t>
+          <t>Evaluating the impact of object-oriented design on software quality</t>
         </is>
       </c>
     </row>
     <row r="709">
       <c r="A709" t="inlineStr">
         <is>
-          <t>Cloud Migration</t>
+          <t>Software Fault Prediction Metrics</t>
         </is>
       </c>
       <c r="B709" t="inlineStr">
         <is>
-          <t>pub.1061541753</t>
+          <t>pub.1038168456</t>
         </is>
       </c>
       <c r="C709" t="inlineStr">
         <is>
-          <t>pub.1043650304</t>
+          <t>pub.1061154182</t>
         </is>
       </c>
       <c r="D709" t="inlineStr">
         <is>
-          <t>A systematic review of effect size in software engineering experiments</t>
+          <t>A validation of object-oriented design metrics as quality indicators</t>
         </is>
       </c>
     </row>
     <row r="710">
       <c r="A710" t="inlineStr">
         <is>
-          <t>Cloud Migration</t>
+          <t>Software Fault Prediction Metrics</t>
         </is>
       </c>
       <c r="B710" t="inlineStr">
         <is>
-          <t>pub.1061541753</t>
+          <t>pub.1038168456</t>
         </is>
       </c>
       <c r="C710" t="inlineStr">
         <is>
-          <t>pub.1017554634</t>
+          <t>pub.1061154197</t>
         </is>
       </c>
       <c r="D710" t="inlineStr">
         <is>
-          <t>Systematic review of organizational motivations for adopting CMM-based SPI</t>
+          <t>Predicting fault-prone software modules in telephone switches</t>
         </is>
       </c>
     </row>
     <row r="711">
       <c r="A711" t="inlineStr">
         <is>
-          <t>Cloud Migration</t>
+          <t>Software Fault Prediction Metrics</t>
         </is>
       </c>
       <c r="B711" t="inlineStr">
         <is>
-          <t>pub.1061541753</t>
+          <t>pub.1038168456</t>
         </is>
       </c>
       <c r="C711" t="inlineStr">
         <is>
-          <t>pub.1000653945</t>
+          <t>pub.1094566044</t>
         </is>
       </c>
       <c r="D711" t="inlineStr">
         <is>
-          <t>Status of Empirical Research in Software Engineering</t>
+          <t>Validation of the coupling dependency metric as a predictor of run-time failures and maintenance measures</t>
         </is>
       </c>
     </row>
     <row r="712">
       <c r="A712" t="inlineStr">
         <is>
-          <t>Cloud Migration</t>
+          <t>Software Fault Prediction Metrics</t>
         </is>
       </c>
       <c r="B712" t="inlineStr">
         <is>
-          <t>pub.1061541753</t>
+          <t>pub.1038168456</t>
         </is>
       </c>
       <c r="C712" t="inlineStr">
         <is>
-          <t>pub.1094400008</t>
+          <t>pub.1094661240</t>
         </is>
       </c>
       <c r="D712" t="inlineStr">
         <is>
-          <t>Software Project Economics: A Roadmap</t>
+          <t>Predicting fault-prone classes with design measures in object-oriented systems</t>
         </is>
       </c>
     </row>
     <row r="713">
       <c r="A713" t="inlineStr">
         <is>
-          <t>Cloud Migration</t>
+          <t>Software Fault Prediction Metrics</t>
         </is>
       </c>
       <c r="B713" t="inlineStr">
         <is>
-          <t>pub.1061541753</t>
+          <t>pub.1038168456</t>
         </is>
       </c>
       <c r="C713" t="inlineStr">
         <is>
-          <t>pub.1013552649</t>
+          <t>pub.1093776808</t>
         </is>
       </c>
       <c r="D713" t="inlineStr">
         <is>
-          <t>Software process improvement in small and medium software enterprises: a systematic review</t>
+          <t>A comprehensive empirical validation of design measures for object-oriented systems</t>
         </is>
       </c>
     </row>
@@ -16132,12 +16132,12 @@
       </c>
       <c r="C714" t="inlineStr">
         <is>
-          <t>pub.1095624517</t>
+          <t>pub.1094303700</t>
         </is>
       </c>
       <c r="D714" t="inlineStr">
         <is>
-          <t>Evaluating the impact of object-oriented design on software quality</t>
+          <t>Code churn: a measure for estimating the impact of code change</t>
         </is>
       </c>
     </row>
@@ -16154,12 +16154,12 @@
       </c>
       <c r="C715" t="inlineStr">
         <is>
-          <t>pub.1061154182</t>
+          <t>pub.1094349395</t>
         </is>
       </c>
       <c r="D715" t="inlineStr">
         <is>
-          <t>A validation of object-oriented design metrics as quality indicators</t>
+          <t>Prediction of fault-proneness at early phase in object-oriented development</t>
         </is>
       </c>
     </row>
@@ -16176,12 +16176,12 @@
       </c>
       <c r="C716" t="inlineStr">
         <is>
-          <t>pub.1061154197</t>
+          <t>pub.1093506486</t>
         </is>
       </c>
       <c r="D716" t="inlineStr">
         <is>
-          <t>Predicting fault-prone software modules in telephone switches</t>
+          <t>An empirical study on object-oriented metrics</t>
         </is>
       </c>
     </row>
@@ -16198,12 +16198,12 @@
       </c>
       <c r="C717" t="inlineStr">
         <is>
-          <t>pub.1094566044</t>
+          <t>pub.1061154618</t>
         </is>
       </c>
       <c r="D717" t="inlineStr">
         <is>
-          <t>Validation of the coupling dependency metric as a predictor of run-time failures and maintenance measures</t>
+          <t>Predicting fault incidence using software change history</t>
         </is>
       </c>
     </row>
@@ -16220,12 +16220,12 @@
       </c>
       <c r="C718" t="inlineStr">
         <is>
-          <t>pub.1094661240</t>
+          <t>pub.1095336786</t>
         </is>
       </c>
       <c r="D718" t="inlineStr">
         <is>
-          <t>Predicting fault-prone classes with design measures in object-oriented systems</t>
+          <t>An application of fuzzy clustering to software quality prediction</t>
         </is>
       </c>
     </row>
@@ -16242,12 +16242,12 @@
       </c>
       <c r="C719" t="inlineStr">
         <is>
-          <t>pub.1093776808</t>
+          <t>pub.1094791278</t>
         </is>
       </c>
       <c r="D719" t="inlineStr">
         <is>
-          <t>A comprehensive empirical validation of design measures for object-oriented systems</t>
+          <t>Using product, process, and execution metrics to predict fault-prone software modules with classification trees</t>
         </is>
       </c>
     </row>
@@ -16264,12 +16264,12 @@
       </c>
       <c r="C720" t="inlineStr">
         <is>
-          <t>pub.1094303700</t>
+          <t>pub.1093396093</t>
         </is>
       </c>
       <c r="D720" t="inlineStr">
         <is>
-          <t>Code churn: a measure for estimating the impact of code change</t>
+          <t>A study on fault-proneness detection of object-oriented systems</t>
         </is>
       </c>
     </row>
@@ -16286,12 +16286,12 @@
       </c>
       <c r="C721" t="inlineStr">
         <is>
-          <t>pub.1094349395</t>
+          <t>pub.1061154750</t>
         </is>
       </c>
       <c r="D721" t="inlineStr">
         <is>
-          <t>Prediction of fault-proneness at early phase in object-oriented development</t>
+          <t>The confounding effect of class size on the validity of object-oriented metrics</t>
         </is>
       </c>
     </row>
@@ -16308,12 +16308,12 @@
       </c>
       <c r="C722" t="inlineStr">
         <is>
-          <t>pub.1093506486</t>
+          <t>pub.1061788213</t>
         </is>
       </c>
       <c r="D722" t="inlineStr">
         <is>
-          <t>An empirical study on object-oriented metrics</t>
+          <t>Assessing the applicability of fault-proneness models across object-oriented software projects</t>
         </is>
       </c>
     </row>
@@ -16330,12 +16330,12 @@
       </c>
       <c r="C723" t="inlineStr">
         <is>
-          <t>pub.1061154618</t>
+          <t>pub.1094902607</t>
         </is>
       </c>
       <c r="D723" t="inlineStr">
         <is>
-          <t>Predicting fault incidence using software change history</t>
+          <t>Metrics That Matter</t>
         </is>
       </c>
     </row>
@@ -16352,12 +16352,12 @@
       </c>
       <c r="C724" t="inlineStr">
         <is>
-          <t>pub.1095336786</t>
+          <t>pub.1093519125</t>
         </is>
       </c>
       <c r="D724" t="inlineStr">
         <is>
-          <t>An application of fuzzy clustering to software quality prediction</t>
+          <t>Predicting fault-proneness using OO metrics. An industrial case study</t>
         </is>
       </c>
     </row>
@@ -16374,12 +16374,12 @@
       </c>
       <c r="C725" t="inlineStr">
         <is>
-          <t>pub.1094791278</t>
+          <t>pub.1094933957</t>
         </is>
       </c>
       <c r="D725" t="inlineStr">
         <is>
-          <t>Using product, process, and execution metrics to predict fault-prone software modules with classification trees</t>
+          <t>How Good is Your Blind Spot Sampling Policy?</t>
         </is>
       </c>
     </row>
@@ -16396,12 +16396,12 @@
       </c>
       <c r="C726" t="inlineStr">
         <is>
-          <t>pub.1093396093</t>
+          <t>pub.1094572706</t>
         </is>
       </c>
       <c r="D726" t="inlineStr">
         <is>
-          <t>A study on fault-proneness detection of object-oriented systems</t>
+          <t>Finding Predictors of Field Defects for Open Source Software Systems in Commonly Available Data Sources: a Case Study of OpenBSD</t>
         </is>
       </c>
     </row>
@@ -16418,12 +16418,12 @@
       </c>
       <c r="C727" t="inlineStr">
         <is>
-          <t>pub.1061154750</t>
+          <t>pub.1061788438</t>
         </is>
       </c>
       <c r="D727" t="inlineStr">
         <is>
-          <t>The confounding effect of class size on the validity of object-oriented metrics</t>
+          <t>Empirical validation of object-oriented metrics on open source software for fault prediction</t>
         </is>
       </c>
     </row>
@@ -16440,12 +16440,12 @@
       </c>
       <c r="C728" t="inlineStr">
         <is>
-          <t>pub.1061788213</t>
+          <t>pub.1005717752</t>
         </is>
       </c>
       <c r="D728" t="inlineStr">
         <is>
-          <t>Assessing the applicability of fault-proneness models across object-oriented software projects</t>
+          <t>Use of relative code churn measures to predict system defect density</t>
         </is>
       </c>
     </row>
@@ -16462,12 +16462,12 @@
       </c>
       <c r="C729" t="inlineStr">
         <is>
-          <t>pub.1094902607</t>
+          <t>pub.1095448393</t>
         </is>
       </c>
       <c r="D729" t="inlineStr">
         <is>
-          <t>Metrics That Matter</t>
+          <t>Can Cohesion Predict Fault Density?</t>
         </is>
       </c>
     </row>
@@ -16484,12 +16484,12 @@
       </c>
       <c r="C730" t="inlineStr">
         <is>
-          <t>pub.1093519125</t>
+          <t>pub.1061788513</t>
         </is>
       </c>
       <c r="D730" t="inlineStr">
         <is>
-          <t>Predicting fault-proneness using OO metrics. An industrial case study</t>
+          <t>Empirical Analysis of Object-Oriented Design Metrics for Predicting High and Low Severity Faults</t>
         </is>
       </c>
     </row>
@@ -16506,12 +16506,12 @@
       </c>
       <c r="C731" t="inlineStr">
         <is>
-          <t>pub.1094933957</t>
+          <t>pub.1093266454</t>
         </is>
       </c>
       <c r="D731" t="inlineStr">
         <is>
-          <t>How Good is Your Blind Spot Sampling Policy?</t>
+          <t>Using Historical In-Process and Product Metrics for Early Estimation of Software Failures</t>
         </is>
       </c>
     </row>
@@ -16528,12 +16528,12 @@
       </c>
       <c r="C732" t="inlineStr">
         <is>
-          <t>pub.1094572706</t>
+          <t>pub.1061788591</t>
         </is>
       </c>
       <c r="D732" t="inlineStr">
         <is>
-          <t>Finding Predictors of Field Defects for Open Source Software Systems in Commonly Available Data Sources: a Case Study of OpenBSD</t>
+          <t>Empirical Validation of Three Software Metrics Suites to Predict Fault-Proneness of Object-Oriented Classes Developed Using Highly Iterative or Agile Software Development Processes</t>
         </is>
       </c>
     </row>
@@ -16550,12 +16550,12 @@
       </c>
       <c r="C733" t="inlineStr">
         <is>
-          <t>pub.1061788438</t>
+          <t>pub.1095418072</t>
         </is>
       </c>
       <c r="D733" t="inlineStr">
         <is>
-          <t>Empirical validation of object-oriented metrics on open source software for fault prediction</t>
+          <t>Predicting Defects for Eclipse</t>
         </is>
       </c>
     </row>
@@ -16572,12 +16572,12 @@
       </c>
       <c r="C734" t="inlineStr">
         <is>
-          <t>pub.1005717752</t>
+          <t>pub.1061788629</t>
         </is>
       </c>
       <c r="D734" t="inlineStr">
         <is>
-          <t>Use of relative code churn measures to predict system defect density</t>
+          <t>Empirical Analysis of Software Fault Content and Fault Proneness Using Bayesian Methods</t>
         </is>
       </c>
     </row>
@@ -16594,12 +16594,12 @@
       </c>
       <c r="C735" t="inlineStr">
         <is>
-          <t>pub.1095448393</t>
+          <t>pub.1093292255</t>
         </is>
       </c>
       <c r="D735" t="inlineStr">
         <is>
-          <t>Can Cohesion Predict Fault Density?</t>
+          <t>Using Software Dependencies and Churn Metrics to Predict Field Failures: An Empirical Case Study</t>
         </is>
       </c>
     </row>
@@ -16616,12 +16616,12 @@
       </c>
       <c r="C736" t="inlineStr">
         <is>
-          <t>pub.1061788513</t>
+          <t>pub.1095355101</t>
         </is>
       </c>
       <c r="D736" t="inlineStr">
         <is>
-          <t>Empirical Analysis of Object-Oriented Design Metrics for Predicting High and Low Severity Faults</t>
+          <t>Fault Prediction using Early Lifecycle Data</t>
         </is>
       </c>
     </row>
@@ -16638,12 +16638,12 @@
       </c>
       <c r="C737" t="inlineStr">
         <is>
-          <t>pub.1093266454</t>
+          <t>pub.1061788604</t>
         </is>
       </c>
       <c r="D737" t="inlineStr">
         <is>
-          <t>Using Historical In-Process and Product Metrics for Early Estimation of Software Failures</t>
+          <t>Data Mining Static Code Attributes to Learn Defect Predictors</t>
         </is>
       </c>
     </row>
@@ -16660,12 +16660,12 @@
       </c>
       <c r="C738" t="inlineStr">
         <is>
-          <t>pub.1061788591</t>
+          <t>pub.1061788656</t>
         </is>
       </c>
       <c r="D738" t="inlineStr">
         <is>
-          <t>Empirical Validation of Three Software Metrics Suites to Predict Fault-Proneness of Object-Oriented Classes Developed Using Highly Iterative or Agile Software Development Processes</t>
+          <t>Using the Conceptual Cohesion of Classes for Fault Prediction in Object-Oriented Systems</t>
         </is>
       </c>
     </row>
@@ -16682,12 +16682,12 @@
       </c>
       <c r="C739" t="inlineStr">
         <is>
-          <t>pub.1095418072</t>
+          <t>pub.1094238526</t>
         </is>
       </c>
       <c r="D739" t="inlineStr">
         <is>
-          <t>Predicting Defects for Eclipse</t>
+          <t>Defect Prediction Using Combined Product and Project Metrics a Case Study from the Open Source “Apache” MyFaces Project Family</t>
         </is>
       </c>
     </row>
@@ -16704,12 +16704,12 @@
       </c>
       <c r="C740" t="inlineStr">
         <is>
-          <t>pub.1061788629</t>
+          <t>pub.1031519727</t>
         </is>
       </c>
       <c r="D740" t="inlineStr">
         <is>
-          <t>Empirical Analysis of Software Fault Content and Fault Proneness Using Bayesian Methods</t>
+          <t>A comparative analysis of the efficiency of change metrics and static code attributes for defect prediction</t>
         </is>
       </c>
     </row>
@@ -16726,12 +16726,12 @@
       </c>
       <c r="C741" t="inlineStr">
         <is>
-          <t>pub.1093292255</t>
+          <t>pub.1048522318</t>
         </is>
       </c>
       <c r="D741" t="inlineStr">
         <is>
-          <t>Using Software Dependencies and Churn Metrics to Predict Field Failures: An Empirical Case Study</t>
+          <t>The influence of organizational structure on software quality</t>
         </is>
       </c>
     </row>
@@ -16748,12 +16748,12 @@
       </c>
       <c r="C742" t="inlineStr">
         <is>
-          <t>pub.1095355101</t>
+          <t>pub.1022710599</t>
         </is>
       </c>
       <c r="D742" t="inlineStr">
         <is>
-          <t>Fault Prediction using Early Lifecycle Data</t>
+          <t>Predicting defects using network analysis on dependency graphs</t>
         </is>
       </c>
     </row>
@@ -16770,12 +16770,12 @@
       </c>
       <c r="C743" t="inlineStr">
         <is>
-          <t>pub.1061788604</t>
+          <t>pub.1095559062</t>
         </is>
       </c>
       <c r="D743" t="inlineStr">
         <is>
-          <t>Data Mining Static Code Attributes to Learn Defect Predictors</t>
+          <t>Evolution and Search Based Metrics to Improve Defects Prediction</t>
         </is>
       </c>
     </row>
@@ -16792,12 +16792,12 @@
       </c>
       <c r="C744" t="inlineStr">
         <is>
-          <t>pub.1061788656</t>
+          <t>pub.1095317546</t>
         </is>
       </c>
       <c r="D744" t="inlineStr">
         <is>
-          <t>Using the Conceptual Cohesion of Classes for Fault Prediction in Object-Oriented Systems</t>
+          <t>Predicting faults using the complexity of code changes</t>
         </is>
       </c>
     </row>
@@ -16814,12 +16814,12 @@
       </c>
       <c r="C745" t="inlineStr">
         <is>
-          <t>pub.1094238526</t>
+          <t>pub.1095132962</t>
         </is>
       </c>
       <c r="D745" t="inlineStr">
         <is>
-          <t>Defect Prediction Using Combined Product and Project Metrics a Case Study from the Open Source “Apache” MyFaces Project Family</t>
+          <t>Predicting Defects in SAP Java Code: An Experience Report</t>
         </is>
       </c>
     </row>
@@ -16836,12 +16836,12 @@
       </c>
       <c r="C746" t="inlineStr">
         <is>
-          <t>pub.1031519727</t>
+          <t>pub.1093362345</t>
         </is>
       </c>
       <c r="D746" t="inlineStr">
         <is>
-          <t>A comparative analysis of the efficiency of change metrics and static code attributes for defect prediction</t>
+          <t>Merits of using repository metrics in defect prediction for open source projects</t>
         </is>
       </c>
     </row>
@@ -16858,12 +16858,12 @@
       </c>
       <c r="C747" t="inlineStr">
         <is>
-          <t>pub.1048522318</t>
+          <t>pub.1094242278</t>
         </is>
       </c>
       <c r="D747" t="inlineStr">
         <is>
-          <t>The influence of organizational structure on software quality</t>
+          <t>An Investigation of the Relationships between Lines of Code and Defects</t>
         </is>
       </c>
     </row>
@@ -16880,12 +16880,12 @@
       </c>
       <c r="C748" t="inlineStr">
         <is>
-          <t>pub.1022710599</t>
+          <t>pub.1094738621</t>
         </is>
       </c>
       <c r="D748" t="inlineStr">
         <is>
-          <t>Predicting defects using network analysis on dependency graphs</t>
+          <t>Ineffectiveness of Use of Software Science Metrics as Predictors of Defects in Object Oriented Software</t>
         </is>
       </c>
     </row>
@@ -16902,12 +16902,12 @@
       </c>
       <c r="C749" t="inlineStr">
         <is>
-          <t>pub.1095559062</t>
+          <t>pub.1093856281</t>
         </is>
       </c>
       <c r="D749" t="inlineStr">
         <is>
-          <t>Evolution and Search Based Metrics to Improve Defects Prediction</t>
+          <t>On the Relationship between Change Coupling and Software Defects</t>
         </is>
       </c>
     </row>
@@ -16924,12 +16924,12 @@
       </c>
       <c r="C750" t="inlineStr">
         <is>
-          <t>pub.1095317546</t>
+          <t>pub.1095496474</t>
         </is>
       </c>
       <c r="D750" t="inlineStr">
         <is>
-          <t>Predicting faults using the complexity of code changes</t>
+          <t>An Extensive Comparison of Bug Prediction Approaches</t>
         </is>
       </c>
     </row>
@@ -16946,12 +16946,12 @@
       </c>
       <c r="C751" t="inlineStr">
         <is>
-          <t>pub.1095132962</t>
+          <t>pub.1094464848</t>
         </is>
       </c>
       <c r="D751" t="inlineStr">
         <is>
-          <t>Predicting Defects in SAP Java Code: An Experience Report</t>
+          <t>Assessing UML Design Metrics for Predicting Fault-prone Classes in a Java System</t>
         </is>
       </c>
     </row>
@@ -16968,12 +16968,12 @@
       </c>
       <c r="C752" t="inlineStr">
         <is>
-          <t>pub.1093362345</t>
+          <t>pub.1093508390</t>
         </is>
       </c>
       <c r="D752" t="inlineStr">
         <is>
-          <t>Merits of using repository metrics in defect prediction for open source projects</t>
+          <t>An Empirical Approach for Software Fault Prediction</t>
         </is>
       </c>
     </row>
@@ -16990,12 +16990,12 @@
       </c>
       <c r="C753" t="inlineStr">
         <is>
-          <t>pub.1094242278</t>
+          <t>pub.1093246157</t>
         </is>
       </c>
       <c r="D753" t="inlineStr">
         <is>
-          <t>An Investigation of the Relationships between Lines of Code and Defects</t>
+          <t>New Conceptual Coupling and Cohesion Metrics for Object-Oriented Systems</t>
         </is>
       </c>
     </row>
@@ -17012,12 +17012,12 @@
       </c>
       <c r="C754" t="inlineStr">
         <is>
-          <t>pub.1094738621</t>
+          <t>pub.1094870261</t>
         </is>
       </c>
       <c r="D754" t="inlineStr">
         <is>
-          <t>Ineffectiveness of Use of Software Science Metrics as Predictors of Defects in Object Oriented Software</t>
+          <t>Change Bursts as Defect Predictors</t>
         </is>
       </c>
     </row>
@@ -17034,144 +17034,120 @@
       </c>
       <c r="C755" t="inlineStr">
         <is>
-          <t>pub.1093856281</t>
+          <t>pub.1093463018</t>
         </is>
       </c>
       <c r="D755" t="inlineStr">
         <is>
-          <t>On the Relationship between Change Coupling and Software Defects</t>
+          <t>An Empirical Study on Object-Oriented Metrics and Software Evolution in order to Reduce Testing Costs by Predicting Change-Prone Classes</t>
         </is>
       </c>
     </row>
     <row r="756">
       <c r="A756" t="inlineStr">
         <is>
-          <t>Software Fault Prediction Metrics</t>
-        </is>
-      </c>
-      <c r="B756" t="inlineStr">
+          <t>Software Defect Prediction</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr"/>
+      <c r="C756" t="inlineStr">
         <is>
           <t>pub.1038168456</t>
         </is>
       </c>
-      <c r="C756" t="inlineStr">
-        <is>
-          <t>pub.1095496474</t>
-        </is>
-      </c>
       <c r="D756" t="inlineStr">
         <is>
-          <t>An Extensive Comparison of Bug Prediction Approaches</t>
+          <t>Software fault prediction metrics: A systematic literature review</t>
         </is>
       </c>
     </row>
     <row r="757">
       <c r="A757" t="inlineStr">
         <is>
-          <t>Software Fault Prediction Metrics</t>
-        </is>
-      </c>
-      <c r="B757" t="inlineStr">
-        <is>
-          <t>pub.1038168456</t>
-        </is>
-      </c>
+          <t>Software Defect Prediction</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr"/>
       <c r="C757" t="inlineStr">
         <is>
-          <t>pub.1094464848</t>
+          <t>pub.1016640320</t>
         </is>
       </c>
       <c r="D757" t="inlineStr">
         <is>
-          <t>Assessing UML Design Metrics for Predicting Fault-prone Classes in a Java System</t>
+          <t>Regression via Classification applied on software defect estimation</t>
         </is>
       </c>
     </row>
     <row r="758">
       <c r="A758" t="inlineStr">
         <is>
-          <t>Software Fault Prediction Metrics</t>
-        </is>
-      </c>
-      <c r="B758" t="inlineStr">
-        <is>
-          <t>pub.1038168456</t>
-        </is>
-      </c>
+          <t>Software Defect Prediction</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr"/>
       <c r="C758" t="inlineStr">
         <is>
-          <t>pub.1093508390</t>
+          <t>pub.1044795300</t>
         </is>
       </c>
       <c r="D758" t="inlineStr">
         <is>
-          <t>An Empirical Approach for Software Fault Prediction</t>
+          <t>Mining software repositories for comprehensible software fault prediction models</t>
         </is>
       </c>
     </row>
     <row r="759">
       <c r="A759" t="inlineStr">
         <is>
-          <t>Software Fault Prediction Metrics</t>
-        </is>
-      </c>
-      <c r="B759" t="inlineStr">
-        <is>
-          <t>pub.1038168456</t>
-        </is>
-      </c>
+          <t>Software Defect Prediction</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr"/>
       <c r="C759" t="inlineStr">
         <is>
-          <t>pub.1093246157</t>
+          <t>pub.1049597330</t>
         </is>
       </c>
       <c r="D759" t="inlineStr">
         <is>
-          <t>New Conceptual Coupling and Cohesion Metrics for Object-Oriented Systems</t>
+          <t>A systematic review of software fault prediction studies</t>
         </is>
       </c>
     </row>
     <row r="760">
       <c r="A760" t="inlineStr">
         <is>
-          <t>Software Fault Prediction Metrics</t>
-        </is>
-      </c>
-      <c r="B760" t="inlineStr">
-        <is>
-          <t>pub.1038168456</t>
-        </is>
-      </c>
+          <t>Software Defect Prediction</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr"/>
       <c r="C760" t="inlineStr">
         <is>
-          <t>pub.1094870261</t>
+          <t>pub.1030311613</t>
         </is>
       </c>
       <c r="D760" t="inlineStr">
         <is>
-          <t>Change Bursts as Defect Predictors</t>
+          <t>Applying machine learning to software fault-proneness prediction</t>
         </is>
       </c>
     </row>
     <row r="761">
       <c r="A761" t="inlineStr">
         <is>
-          <t>Software Fault Prediction Metrics</t>
-        </is>
-      </c>
-      <c r="B761" t="inlineStr">
-        <is>
-          <t>pub.1038168456</t>
-        </is>
-      </c>
+          <t>Software Defect Prediction</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr"/>
       <c r="C761" t="inlineStr">
         <is>
-          <t>pub.1093463018</t>
+          <t>pub.1030916580</t>
         </is>
       </c>
       <c r="D761" t="inlineStr">
         <is>
-          <t>An Empirical Study on Object-Oriented Metrics and Software Evolution in order to Reduce Testing Costs by Predicting Change-Prone Classes</t>
+          <t>Predicting defect-prone software modules using support vector machines</t>
         </is>
       </c>
     </row>
@@ -17184,12 +17160,12 @@
       <c r="B762" t="inlineStr"/>
       <c r="C762" t="inlineStr">
         <is>
-          <t>pub.1038168456</t>
+          <t>pub.1061798146</t>
         </is>
       </c>
       <c r="D762" t="inlineStr">
         <is>
-          <t>Software fault prediction metrics: A systematic literature review</t>
+          <t>Empirical Case Studies in Attribute Noise Detection</t>
         </is>
       </c>
     </row>
@@ -17202,12 +17178,12 @@
       <c r="B763" t="inlineStr"/>
       <c r="C763" t="inlineStr">
         <is>
-          <t>pub.1016640320</t>
+          <t>pub.1095749524</t>
         </is>
       </c>
       <c r="D763" t="inlineStr">
         <is>
-          <t>Regression via Classification applied on software defect estimation</t>
+          <t>Feature Selection with Imbalanced Data for Software Defect Prediction</t>
         </is>
       </c>
     </row>
@@ -17220,12 +17196,12 @@
       <c r="B764" t="inlineStr"/>
       <c r="C764" t="inlineStr">
         <is>
-          <t>pub.1044795300</t>
+          <t>pub.1040067116</t>
         </is>
       </c>
       <c r="D764" t="inlineStr">
         <is>
-          <t>Mining software repositories for comprehensible software fault prediction models</t>
+          <t>Investigating the effect of dataset size, metrics sets, and feature selection techniques on software fault prediction problem</t>
         </is>
       </c>
     </row>
@@ -17238,12 +17214,12 @@
       <c r="B765" t="inlineStr"/>
       <c r="C765" t="inlineStr">
         <is>
-          <t>pub.1049597330</t>
+          <t>pub.1016659627</t>
         </is>
       </c>
       <c r="D765" t="inlineStr">
         <is>
-          <t>A systematic review of software fault prediction studies</t>
+          <t>On the relative value of cross-company and within-company data for defect prediction</t>
         </is>
       </c>
     </row>
@@ -17256,12 +17232,12 @@
       <c r="B766" t="inlineStr"/>
       <c r="C766" t="inlineStr">
         <is>
-          <t>pub.1030311613</t>
+          <t>pub.1032338646</t>
         </is>
       </c>
       <c r="D766" t="inlineStr">
         <is>
-          <t>Applying machine learning to software fault-proneness prediction</t>
+          <t>Data mining source code for locating software bugs: A case study in telecommunication industry</t>
         </is>
       </c>
     </row>
@@ -17274,12 +17250,12 @@
       <c r="B767" t="inlineStr"/>
       <c r="C767" t="inlineStr">
         <is>
-          <t>pub.1030916580</t>
+          <t>pub.1061788822</t>
         </is>
       </c>
       <c r="D767" t="inlineStr">
         <is>
-          <t>Predicting defect-prone software modules using support vector machines</t>
+          <t>Evolutionary Optimization of Software Quality Modeling with Multiple Repositories</t>
         </is>
       </c>
     </row>
@@ -17292,12 +17268,12 @@
       <c r="B768" t="inlineStr"/>
       <c r="C768" t="inlineStr">
         <is>
-          <t>pub.1061798146</t>
+          <t>pub.1009020017</t>
         </is>
       </c>
       <c r="D768" t="inlineStr">
         <is>
-          <t>Empirical Case Studies in Attribute Noise Detection</t>
+          <t>Cost-sensitive boosting neural networks for software defect prediction</t>
         </is>
       </c>
     </row>
@@ -17310,12 +17286,12 @@
       <c r="B769" t="inlineStr"/>
       <c r="C769" t="inlineStr">
         <is>
-          <t>pub.1095749524</t>
+          <t>pub.1006992827</t>
         </is>
       </c>
       <c r="D769" t="inlineStr">
         <is>
-          <t>Feature Selection with Imbalanced Data for Software Defect Prediction</t>
+          <t>Defect prediction from static code features: current results, limitations, new approaches</t>
         </is>
       </c>
     </row>
@@ -17328,12 +17304,12 @@
       <c r="B770" t="inlineStr"/>
       <c r="C770" t="inlineStr">
         <is>
-          <t>pub.1040067116</t>
+          <t>pub.1029996552</t>
         </is>
       </c>
       <c r="D770" t="inlineStr">
         <is>
-          <t>Investigating the effect of dataset size, metrics sets, and feature selection techniques on software fault prediction problem</t>
+          <t>A systematic and comprehensive investigation of methods to build and evaluate fault prediction models</t>
         </is>
       </c>
     </row>
@@ -17346,12 +17322,12 @@
       <c r="B771" t="inlineStr"/>
       <c r="C771" t="inlineStr">
         <is>
-          <t>pub.1016659627</t>
+          <t>pub.1093583251</t>
         </is>
       </c>
       <c r="D771" t="inlineStr">
         <is>
-          <t>On the relative value of cross-company and within-company data for defect prediction</t>
+          <t>A Comparative Study of Ensemble Feature Selection Techniques for Software Defect Prediction</t>
         </is>
       </c>
     </row>
@@ -17364,12 +17340,12 @@
       <c r="B772" t="inlineStr"/>
       <c r="C772" t="inlineStr">
         <is>
-          <t>pub.1032338646</t>
+          <t>pub.1061788851</t>
         </is>
       </c>
       <c r="D772" t="inlineStr">
         <is>
-          <t>Data mining source code for locating software bugs: A case study in telecommunication industry</t>
+          <t>A General Software Defect-Proneness Prediction Framework</t>
         </is>
       </c>
     </row>
@@ -17382,12 +17358,12 @@
       <c r="B773" t="inlineStr"/>
       <c r="C773" t="inlineStr">
         <is>
-          <t>pub.1061788822</t>
+          <t>pub.1050027319</t>
         </is>
       </c>
       <c r="D773" t="inlineStr">
         <is>
-          <t>Evolutionary Optimization of Software Quality Modeling with Multiple Repositories</t>
+          <t>Practical development of an Eclipse-based software fault prediction tool using Naive Bayes algorithm</t>
         </is>
       </c>
     </row>
@@ -17400,12 +17376,12 @@
       <c r="B774" t="inlineStr"/>
       <c r="C774" t="inlineStr">
         <is>
-          <t>pub.1009020017</t>
+          <t>pub.1061795697</t>
         </is>
       </c>
       <c r="D774" t="inlineStr">
         <is>
-          <t>Cost-sensitive boosting neural networks for software defect prediction</t>
+          <t>Comparing Boosting and Bagging Techniques with Noisy and Imbalanced Data</t>
         </is>
       </c>
     </row>
@@ -17418,12 +17394,12 @@
       <c r="B775" t="inlineStr"/>
       <c r="C775" t="inlineStr">
         <is>
-          <t>pub.1006992827</t>
+          <t>pub.1026182535</t>
         </is>
       </c>
       <c r="D775" t="inlineStr">
         <is>
-          <t>Defect prediction from static code features: current results, limitations, new approaches</t>
+          <t>An industrial case study of classifier ensembles for locating software defects</t>
         </is>
       </c>
     </row>
@@ -17436,12 +17412,12 @@
       <c r="B776" t="inlineStr"/>
       <c r="C776" t="inlineStr">
         <is>
-          <t>pub.1029996552</t>
+          <t>pub.1014268670</t>
         </is>
       </c>
       <c r="D776" t="inlineStr">
         <is>
-          <t>A systematic and comprehensive investigation of methods to build and evaluate fault prediction models</t>
+          <t>An ant colony optimization algorithm to improve software quality prediction models: Case of class stability</t>
         </is>
       </c>
     </row>
@@ -17454,12 +17430,12 @@
       <c r="B777" t="inlineStr"/>
       <c r="C777" t="inlineStr">
         <is>
-          <t>pub.1093583251</t>
+          <t>pub.1061662354</t>
         </is>
       </c>
       <c r="D777" t="inlineStr">
         <is>
-          <t>A Comparative Study of Ensemble Feature Selection Techniques for Software Defect Prediction</t>
+          <t>Software Fault Prediction Using Quad Tree-Based K-Means Clustering Algorithm</t>
         </is>
       </c>
     </row>
@@ -17472,12 +17448,12 @@
       <c r="B778" t="inlineStr"/>
       <c r="C778" t="inlineStr">
         <is>
-          <t>pub.1061788851</t>
+          <t>pub.1061783611</t>
         </is>
       </c>
       <c r="D778" t="inlineStr">
         <is>
-          <t>A General Software Defect-Proneness Prediction Framework</t>
+          <t>Evaluating Stratification Alternatives to Improve Software Defect Prediction</t>
         </is>
       </c>
     </row>
@@ -17490,12 +17466,12 @@
       <c r="B779" t="inlineStr"/>
       <c r="C779" t="inlineStr">
         <is>
-          <t>pub.1050027319</t>
+          <t>pub.1056837147</t>
         </is>
       </c>
       <c r="D779" t="inlineStr">
         <is>
-          <t>Practical development of an Eclipse-based software fault prediction tool using Naive Bayes algorithm</t>
+          <t>Artificial neural network-based metric selection for software fault-prone prediction model</t>
         </is>
       </c>
     </row>
@@ -17508,12 +17484,12 @@
       <c r="B780" t="inlineStr"/>
       <c r="C780" t="inlineStr">
         <is>
-          <t>pub.1061795697</t>
+          <t>pub.1061798471</t>
         </is>
       </c>
       <c r="D780" t="inlineStr">
         <is>
-          <t>Comparing Boosting and Bagging Techniques with Noisy and Imbalanced Data</t>
+          <t>Using Coding-Based Ensemble Learning to Improve Software Defect Prediction</t>
         </is>
       </c>
     </row>
@@ -17526,12 +17502,12 @@
       <c r="B781" t="inlineStr"/>
       <c r="C781" t="inlineStr">
         <is>
-          <t>pub.1026182535</t>
+          <t>pub.1056837144</t>
         </is>
       </c>
       <c r="D781" t="inlineStr">
         <is>
-          <t>An industrial case study of classifier ensembles for locating software defects</t>
+          <t>Reflections on the NASA MDP data sets</t>
         </is>
       </c>
     </row>
@@ -17544,12 +17520,12 @@
       <c r="B782" t="inlineStr"/>
       <c r="C782" t="inlineStr">
         <is>
-          <t>pub.1014268670</t>
+          <t>pub.1041664266</t>
         </is>
       </c>
       <c r="D782" t="inlineStr">
         <is>
-          <t>An ant colony optimization algorithm to improve software quality prediction models: Case of class stability</t>
+          <t>Transfer learning for cross-company software defect prediction</t>
         </is>
       </c>
     </row>
@@ -17562,12 +17538,12 @@
       <c r="B783" t="inlineStr"/>
       <c r="C783" t="inlineStr">
         <is>
-          <t>pub.1061662354</t>
+          <t>pub.1027402804</t>
         </is>
       </c>
       <c r="D783" t="inlineStr">
         <is>
-          <t>Software Fault Prediction Using Quad Tree-Based K-Means Clustering Algorithm</t>
+          <t>User preferences based software defect detection algorithms selection using MCDM</t>
         </is>
       </c>
     </row>
@@ -17580,12 +17556,12 @@
       <c r="B784" t="inlineStr"/>
       <c r="C784" t="inlineStr">
         <is>
-          <t>pub.1061783611</t>
+          <t>pub.1061783588</t>
         </is>
       </c>
       <c r="D784" t="inlineStr">
         <is>
-          <t>Evaluating Stratification Alternatives to Improve Software Defect Prediction</t>
+          <t>Effective Software Fault Localization Using an RBF Neural Network</t>
         </is>
       </c>
     </row>
@@ -17598,12 +17574,12 @@
       <c r="B785" t="inlineStr"/>
       <c r="C785" t="inlineStr">
         <is>
-          <t>pub.1056837147</t>
+          <t>pub.1093218381</t>
         </is>
       </c>
       <c r="D785" t="inlineStr">
         <is>
-          <t>Artificial neural network-based metric selection for software fault-prone prediction model</t>
+          <t>Software Fault Prediction Based on Grey Neural Network</t>
         </is>
       </c>
     </row>
@@ -17616,12 +17592,12 @@
       <c r="B786" t="inlineStr"/>
       <c r="C786" t="inlineStr">
         <is>
-          <t>pub.1061798471</t>
+          <t>pub.1061788960</t>
         </is>
       </c>
       <c r="D786" t="inlineStr">
         <is>
-          <t>Using Coding-Based Ensemble Learning to Improve Software Defect Prediction</t>
+          <t>Toward Comprehensible Software Fault Prediction Models Using Bayesian Network Classifiers</t>
         </is>
       </c>
     </row>
@@ -17634,12 +17610,12 @@
       <c r="B787" t="inlineStr"/>
       <c r="C787" t="inlineStr">
         <is>
-          <t>pub.1056837144</t>
+          <t>pub.1061789009</t>
         </is>
       </c>
       <c r="D787" t="inlineStr">
         <is>
-          <t>Reflections on the NASA MDP data sets</t>
+          <t>Data Quality: Some Comments on the NASA Software Defect Datasets</t>
         </is>
       </c>
     </row>
@@ -17652,12 +17628,12 @@
       <c r="B788" t="inlineStr"/>
       <c r="C788" t="inlineStr">
         <is>
-          <t>pub.1041664266</t>
+          <t>pub.1061783724</t>
         </is>
       </c>
       <c r="D788" t="inlineStr">
         <is>
-          <t>Transfer learning for cross-company software defect prediction</t>
+          <t>Using Class Imbalance Learning for Software Defect Prediction</t>
         </is>
       </c>
     </row>
@@ -17670,12 +17646,12 @@
       <c r="B789" t="inlineStr"/>
       <c r="C789" t="inlineStr">
         <is>
-          <t>pub.1027402804</t>
+          <t>pub.1014545963</t>
         </is>
       </c>
       <c r="D789" t="inlineStr">
         <is>
-          <t>User preferences based software defect detection algorithms selection using MCDM</t>
+          <t>The design of polynomial function-based neural network predictors for detection of software defects</t>
         </is>
       </c>
     </row>
@@ -17688,12 +17664,12 @@
       <c r="B790" t="inlineStr"/>
       <c r="C790" t="inlineStr">
         <is>
-          <t>pub.1061783588</t>
+          <t>pub.1061789060</t>
         </is>
       </c>
       <c r="D790" t="inlineStr">
         <is>
-          <t>Effective Software Fault Localization Using an RBF Neural Network</t>
+          <t>Balancing Privacy and Utility in Cross-Company Defect Prediction</t>
         </is>
       </c>
     </row>
@@ -17706,12 +17682,12 @@
       <c r="B791" t="inlineStr"/>
       <c r="C791" t="inlineStr">
         <is>
-          <t>pub.1093218381</t>
+          <t>pub.1028857888</t>
         </is>
       </c>
       <c r="D791" t="inlineStr">
         <is>
-          <t>Software Fault Prediction Based on Grey Neural Network</t>
+          <t>An empirical comparison and characterization of high defect and high complexity modules</t>
         </is>
       </c>
     </row>
@@ -17724,12 +17700,12 @@
       <c r="B792" t="inlineStr"/>
       <c r="C792" t="inlineStr">
         <is>
-          <t>pub.1061788960</t>
+          <t>pub.1093454342</t>
         </is>
       </c>
       <c r="D792" t="inlineStr">
         <is>
-          <t>Toward Comprehensible Software Fault Prediction Models Using Bayesian Network Classifiers</t>
+          <t>Extract Rules from Software Quality Prediction Model Based on Neural Network</t>
         </is>
       </c>
     </row>
@@ -17742,12 +17718,12 @@
       <c r="B793" t="inlineStr"/>
       <c r="C793" t="inlineStr">
         <is>
-          <t>pub.1061789009</t>
+          <t>pub.1042524665</t>
         </is>
       </c>
       <c r="D793" t="inlineStr">
         <is>
-          <t>Data Quality: Some Comments on the NASA Software Defect Datasets</t>
+          <t>Object oriented software quality prediction using general regression neural networks</t>
         </is>
       </c>
     </row>
@@ -17760,12 +17736,12 @@
       <c r="B794" t="inlineStr"/>
       <c r="C794" t="inlineStr">
         <is>
-          <t>pub.1061783724</t>
+          <t>pub.1061788479</t>
         </is>
       </c>
       <c r="D794" t="inlineStr">
         <is>
-          <t>Using Class Imbalance Learning for Software Defect Prediction</t>
+          <t>Predicting the location and number of faults in large software systems</t>
         </is>
       </c>
     </row>
@@ -17778,12 +17754,12 @@
       <c r="B795" t="inlineStr"/>
       <c r="C795" t="inlineStr">
         <is>
-          <t>pub.1014545963</t>
+          <t>pub.1094284227</t>
         </is>
       </c>
       <c r="D795" t="inlineStr">
         <is>
-          <t>The design of polynomial function-based neural network predictors for detection of software defects</t>
+          <t>A Novel Method for Early Software Quality Prediction Based on Support Vector Machine</t>
         </is>
       </c>
     </row>
@@ -17796,12 +17772,12 @@
       <c r="B796" t="inlineStr"/>
       <c r="C796" t="inlineStr">
         <is>
-          <t>pub.1061789060</t>
+          <t>pub.1093778985</t>
         </is>
       </c>
       <c r="D796" t="inlineStr">
         <is>
-          <t>Balancing Privacy and Utility in Cross-Company Defect Prediction</t>
+          <t>Empirical Assessment of Machine Learning based Software Defect Prediction Techniques</t>
         </is>
       </c>
     </row>
@@ -17814,12 +17790,12 @@
       <c r="B797" t="inlineStr"/>
       <c r="C797" t="inlineStr">
         <is>
-          <t>pub.1028857888</t>
+          <t>pub.1011990728</t>
         </is>
       </c>
       <c r="D797" t="inlineStr">
         <is>
-          <t>An empirical comparison and characterization of high defect and high complexity modules</t>
+          <t>An investigation of the effect of module size on defect prediction using static measures</t>
         </is>
       </c>
     </row>
@@ -17832,12 +17808,12 @@
       <c r="B798" t="inlineStr"/>
       <c r="C798" t="inlineStr">
         <is>
-          <t>pub.1093454342</t>
+          <t>pub.1048561887</t>
         </is>
       </c>
       <c r="D798" t="inlineStr">
         <is>
-          <t>Extract Rules from Software Quality Prediction Model Based on Neural Network</t>
+          <t>Assessment of a New Three-Group Software Quality Classification Technique: An Empirical Case Study</t>
         </is>
       </c>
     </row>
@@ -17850,12 +17826,12 @@
       <c r="B799" t="inlineStr"/>
       <c r="C799" t="inlineStr">
         <is>
-          <t>pub.1042524665</t>
+          <t>pub.1061788527</t>
         </is>
       </c>
       <c r="D799" t="inlineStr">
         <is>
-          <t>Object oriented software quality prediction using general regression neural networks</t>
+          <t>Software defect association mining and defect correction effort prediction</t>
         </is>
       </c>
     </row>
@@ -17868,12 +17844,12 @@
       <c r="B800" t="inlineStr"/>
       <c r="C800" t="inlineStr">
         <is>
-          <t>pub.1061788479</t>
+          <t>pub.1061788513</t>
         </is>
       </c>
       <c r="D800" t="inlineStr">
         <is>
-          <t>Predicting the location and number of faults in large software systems</t>
+          <t>Empirical Analysis of Object-Oriented Design Metrics for Predicting High and Low Severity Faults</t>
         </is>
       </c>
     </row>
@@ -17886,12 +17862,12 @@
       <c r="B801" t="inlineStr"/>
       <c r="C801" t="inlineStr">
         <is>
-          <t>pub.1094284227</t>
+          <t>pub.1094706654</t>
         </is>
       </c>
       <c r="D801" t="inlineStr">
         <is>
-          <t>A Novel Method for Early Software Quality Prediction Based on Support Vector Machine</t>
+          <t>A Unified Framework for Defect Data Analysis Using the MBR Technique</t>
         </is>
       </c>
     </row>
@@ -17904,12 +17880,12 @@
       <c r="B802" t="inlineStr"/>
       <c r="C802" t="inlineStr">
         <is>
-          <t>pub.1093778985</t>
+          <t>pub.1031601770</t>
         </is>
       </c>
       <c r="D802" t="inlineStr">
         <is>
-          <t>Empirical Assessment of Machine Learning based Software Defect Prediction Techniques</t>
+          <t>An empirical study of predicting software faults with case-based reasoning</t>
         </is>
       </c>
     </row>
@@ -17922,12 +17898,12 @@
       <c r="B803" t="inlineStr"/>
       <c r="C803" t="inlineStr">
         <is>
-          <t>pub.1011990728</t>
+          <t>pub.1061788604</t>
         </is>
       </c>
       <c r="D803" t="inlineStr">
         <is>
-          <t>An investigation of the effect of module size on defect prediction using static measures</t>
+          <t>Data Mining Static Code Attributes to Learn Defect Predictors</t>
         </is>
       </c>
     </row>
@@ -17940,12 +17916,12 @@
       <c r="B804" t="inlineStr"/>
       <c r="C804" t="inlineStr">
         <is>
-          <t>pub.1048561887</t>
+          <t>pub.1061795230</t>
         </is>
       </c>
       <c r="D804" t="inlineStr">
         <is>
-          <t>Assessment of a New Three-Group Software Quality Classification Technique: An Empirical Case Study</t>
+          <t>Software Quality Analysis of Unlabeled Program Modules with Semisupervised Clustering</t>
         </is>
       </c>
     </row>
@@ -17958,12 +17934,12 @@
       <c r="B805" t="inlineStr"/>
       <c r="C805" t="inlineStr">
         <is>
-          <t>pub.1061788527</t>
+          <t>pub.1095092354</t>
         </is>
       </c>
       <c r="D805" t="inlineStr">
         <is>
-          <t>Software defect association mining and defect correction effort prediction</t>
+          <t>A practical method for the software fault-prediction</t>
         </is>
       </c>
     </row>
@@ -17976,12 +17952,12 @@
       <c r="B806" t="inlineStr"/>
       <c r="C806" t="inlineStr">
         <is>
-          <t>pub.1061788513</t>
+          <t>pub.1053284993</t>
         </is>
       </c>
       <c r="D806" t="inlineStr">
         <is>
-          <t>Empirical Analysis of Object-Oriented Design Metrics for Predicting High and Low Severity Faults</t>
+          <t>Predicting software defects in varying development lifecycles using Bayesian nets</t>
         </is>
       </c>
     </row>
@@ -17994,12 +17970,12 @@
       <c r="B807" t="inlineStr"/>
       <c r="C807" t="inlineStr">
         <is>
-          <t>pub.1094706654</t>
+          <t>pub.1012487871</t>
         </is>
       </c>
       <c r="D807" t="inlineStr">
         <is>
-          <t>A Unified Framework for Defect Data Analysis Using the MBR Technique</t>
+          <t>Identifying and characterizing change-prone classes in two large-scale open-source products</t>
         </is>
       </c>
     </row>
@@ -18012,12 +17988,12 @@
       <c r="B808" t="inlineStr"/>
       <c r="C808" t="inlineStr">
         <is>
-          <t>pub.1031601770</t>
+          <t>pub.1061788629</t>
         </is>
       </c>
       <c r="D808" t="inlineStr">
         <is>
-          <t>An empirical study of predicting software faults with case-based reasoning</t>
+          <t>Empirical Analysis of Software Fault Content and Fault Proneness Using Bayesian Methods</t>
         </is>
       </c>
     </row>
@@ -18030,118 +18006,10 @@
       <c r="B809" t="inlineStr"/>
       <c r="C809" t="inlineStr">
         <is>
-          <t>pub.1061788604</t>
+          <t>pub.1061788688</t>
         </is>
       </c>
       <c r="D809" t="inlineStr">
-        <is>
-          <t>Data Mining Static Code Attributes to Learn Defect Predictors</t>
-        </is>
-      </c>
-    </row>
-    <row r="810">
-      <c r="A810" t="inlineStr">
-        <is>
-          <t>Software Defect Prediction</t>
-        </is>
-      </c>
-      <c r="B810" t="inlineStr"/>
-      <c r="C810" t="inlineStr">
-        <is>
-          <t>pub.1061795230</t>
-        </is>
-      </c>
-      <c r="D810" t="inlineStr">
-        <is>
-          <t>Software Quality Analysis of Unlabeled Program Modules with Semisupervised Clustering</t>
-        </is>
-      </c>
-    </row>
-    <row r="811">
-      <c r="A811" t="inlineStr">
-        <is>
-          <t>Software Defect Prediction</t>
-        </is>
-      </c>
-      <c r="B811" t="inlineStr"/>
-      <c r="C811" t="inlineStr">
-        <is>
-          <t>pub.1095092354</t>
-        </is>
-      </c>
-      <c r="D811" t="inlineStr">
-        <is>
-          <t>A practical method for the software fault-prediction</t>
-        </is>
-      </c>
-    </row>
-    <row r="812">
-      <c r="A812" t="inlineStr">
-        <is>
-          <t>Software Defect Prediction</t>
-        </is>
-      </c>
-      <c r="B812" t="inlineStr"/>
-      <c r="C812" t="inlineStr">
-        <is>
-          <t>pub.1053284993</t>
-        </is>
-      </c>
-      <c r="D812" t="inlineStr">
-        <is>
-          <t>Predicting software defects in varying development lifecycles using Bayesian nets</t>
-        </is>
-      </c>
-    </row>
-    <row r="813">
-      <c r="A813" t="inlineStr">
-        <is>
-          <t>Software Defect Prediction</t>
-        </is>
-      </c>
-      <c r="B813" t="inlineStr"/>
-      <c r="C813" t="inlineStr">
-        <is>
-          <t>pub.1012487871</t>
-        </is>
-      </c>
-      <c r="D813" t="inlineStr">
-        <is>
-          <t>Identifying and characterizing change-prone classes in two large-scale open-source products</t>
-        </is>
-      </c>
-    </row>
-    <row r="814">
-      <c r="A814" t="inlineStr">
-        <is>
-          <t>Software Defect Prediction</t>
-        </is>
-      </c>
-      <c r="B814" t="inlineStr"/>
-      <c r="C814" t="inlineStr">
-        <is>
-          <t>pub.1061788629</t>
-        </is>
-      </c>
-      <c r="D814" t="inlineStr">
-        <is>
-          <t>Empirical Analysis of Software Fault Content and Fault Proneness Using Bayesian Methods</t>
-        </is>
-      </c>
-    </row>
-    <row r="815">
-      <c r="A815" t="inlineStr">
-        <is>
-          <t>Software Defect Prediction</t>
-        </is>
-      </c>
-      <c r="B815" t="inlineStr"/>
-      <c r="C815" t="inlineStr">
-        <is>
-          <t>pub.1061788688</t>
-        </is>
-      </c>
-      <c r="D815" t="inlineStr">
         <is>
           <t>Benchmarking Classification Models for Software Defect Prediction: A Proposed Framework and Novel Findings</t>
         </is>

</xml_diff>